<commit_message>
multiply matrices transposed (results)
</commit_message>
<xml_diff>
--- a/results/Benchmarks.xlsx
+++ b/results/Benchmarks.xlsx
@@ -201,7 +201,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -573,11 +573,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="99321110"/>
-        <c:axId val="85026599"/>
+        <c:axId val="71456250"/>
+        <c:axId val="85616181"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99321110"/>
+        <c:axId val="71456250"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,7 +605,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85026599"/>
+        <c:crossAx val="85616181"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -613,7 +613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85026599"/>
+        <c:axId val="85616181"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,7 +650,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99321110"/>
+        <c:crossAx val="71456250"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -698,7 +698,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -769,30 +769,36 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>benchmarks!$B$24:$B$30</c:f>
+              <c:f>benchmarks!$B$24:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>476</c:v>
+                  <c:v>807</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1505</c:v>
+                  <c:v>1357</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3608</c:v>
+                  <c:v>1788</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7488</c:v>
+                  <c:v>3104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14585</c:v>
+                  <c:v>4117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23720</c:v>
+                  <c:v>6722</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -860,30 +866,36 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>benchmarks!$C$24:$C$30</c:f>
+              <c:f>benchmarks!$C$24:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>110</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>468</c:v>
+                  <c:v>478</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1477</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3600</c:v>
+                  <c:v>1033</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7467</c:v>
+                  <c:v>1348</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13836</c:v>
+                  <c:v>1755</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23592</c:v>
+                  <c:v>2279</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2838</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -898,11 +910,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="11995940"/>
-        <c:axId val="14950899"/>
+        <c:axId val="15623128"/>
+        <c:axId val="41125205"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="11995940"/>
+        <c:axId val="15623128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,7 +942,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14950899"/>
+        <c:crossAx val="41125205"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -938,7 +950,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14950899"/>
+        <c:axId val="41125205"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,7 +987,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11995940"/>
+        <c:crossAx val="15623128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1027,16 +1039,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>271800</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>31680</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>755280</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>431640</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>735480</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1044,8 +1056,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5970240" y="356760"/>
-        <a:ext cx="5044320" cy="2837160"/>
+        <a:off x="4825800" y="114840"/>
+        <a:ext cx="5678640" cy="3193920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1057,16 +1069,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>203040</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>131400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>801360</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>102960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>264240</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
+      <xdr:colOff>48240</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1074,7 +1086,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4273560" y="3545280"/>
+        <a:off x="4057560" y="3679200"/>
         <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
@@ -1093,7 +1105,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1352,79 +1364,101 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>104</v>
+        <v>669</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>110</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>150</v>
+        <v>800</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>476</v>
+        <v>807</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>468</v>
+        <v>478</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>200</v>
+        <v>900</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>1505</v>
+        <v>1357</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>1477</v>
+        <v>700</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>3608</v>
+        <v>1788</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>3600</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>300</v>
+        <v>1100</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>7488</v>
+        <v>3104</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>7467</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>350</v>
+        <v>1200</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>14585</v>
+        <v>4117</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>13836</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>400</v>
+        <v>1300</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>23720</v>
+        <v>6722</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>23592</v>
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>9235</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>2838</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>14018</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>3431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>